<commit_message>
Final Update (i  hope)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,12 +429,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Modèle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Score</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Moyenne</t>
         </is>
       </c>
     </row>
@@ -446,11 +446,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.8414592146873474</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+          <t>Factuality and Readability</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.8414592146873474 / 2</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>0.8958436548709869</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -461,7 +469,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.9502280950546265</t>
+          <t>Factuality and Readability</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.9502280950546265 / 2</t>
         </is>
       </c>
     </row>

</xml_diff>